<commit_message>
Did an Alt, no GROUPBY
</commit_message>
<xml_diff>
--- a/CH-96 Top Products.xlsx
+++ b/CH-96 Top Products.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19F99536-1B9E-419B-A259-9A43C1F93262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="8_{19F99536-1B9E-419B-A259-9A43C1F93262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2A145DE-BD10-4E9D-9D23-478D6D52AE62}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="Alt1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt1'!$B$2:$D$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$D$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$D$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,8 +42,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="16">
   <si>
     <t>Result</t>
   </si>
@@ -81,6 +107,12 @@
   </si>
   <si>
     <t>% of Month sales</t>
+  </si>
+  <si>
+    <t>Unique Months</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/feed/update/urn:li:activity:7228505467411427329/</t>
   </si>
 </sst>
 </file>
@@ -215,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -251,6 +283,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -350,15 +386,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
+      <xdr:colOff>215900</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>7552</xdr:rowOff>
+      <xdr:rowOff>10726</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1485900</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -373,8 +409,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3057525" y="7552"/>
-          <a:ext cx="4162425" cy="4212023"/>
+          <a:off x="3054350" y="10726"/>
+          <a:ext cx="4165600" cy="4161223"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -491,6 +527,163 @@
         <a:xfrm rot="16200000">
           <a:off x="2591753" y="1743075"/>
           <a:ext cx="519927" cy="451983"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:endParaRPr lang="en-AU" sz="2800" b="0">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>3175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>231775</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Arrow: Bent 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28B8D897-606D-4A92-AA4E-C18AFCEF3818}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="7373937" y="1890713"/>
+          <a:ext cx="860425" cy="1282700"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:endParaRPr lang="en-AU" sz="2800" b="0">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>612775</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>134303</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>245608</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>101780</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Arrow: Down 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{716469C2-3697-4CA9-9D76-F4148E0BCBFD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="2602865" y="1719263"/>
+          <a:ext cx="513577" cy="448808"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
           <a:avLst/>
@@ -798,10 +991,915 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P12" sqref="O12:P12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.75" customWidth="1"/>
+    <col min="5" max="5" width="6.25" customWidth="1"/>
+    <col min="6" max="7" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" customWidth="1"/>
+    <col min="9" max="9" width="11.58203125" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.58203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="I1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="N1" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4"/>
+      <c r="B2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4"/>
+      <c r="B3" s="7">
+        <v>45377</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="8">
+        <v>67</v>
+      </c>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="I3" s="6">
+        <v>3</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="12">
+        <v>0.5234375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4"/>
+      <c r="B4" s="7">
+        <v>45380</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="8">
+        <v>16</v>
+      </c>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="I4" s="6">
+        <v>3</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="12">
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4"/>
+      <c r="B5" s="7">
+        <v>45380</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="8">
+        <v>21</v>
+      </c>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="I5" s="6">
+        <v>3</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="12">
+        <v>0.2890625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4"/>
+      <c r="B6" s="7">
+        <v>45382</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="8">
+        <v>24</v>
+      </c>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="I6" s="6">
+        <v>4</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="12">
+        <v>0.30456852791878175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4"/>
+      <c r="B7" s="7">
+        <v>45383</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="8">
+        <v>30</v>
+      </c>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="I7" s="6">
+        <v>4</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="12">
+        <v>0.23604060913705585</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B8" s="7">
+        <v>45385</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="8">
+        <v>21</v>
+      </c>
+      <c r="I8" s="6">
+        <v>4</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="12">
+        <v>0.45939086294416243</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B9" s="7">
+        <v>45392</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="8">
+        <v>39</v>
+      </c>
+      <c r="I9" s="6">
+        <v>5</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="12">
+        <v>0.6376811594202898</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B10" s="7">
+        <v>45401</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="8">
+        <v>81</v>
+      </c>
+      <c r="I10" s="6">
+        <v>5</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="12">
+        <v>0.32463768115942027</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B11" s="7">
+        <v>45409</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="8">
+        <v>81</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="6">
+        <v>5</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="12">
+        <v>3.7681159420289857E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B12" s="7">
+        <v>45409</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="8">
+        <v>93</v>
+      </c>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B13" s="7">
+        <v>45410</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="8">
+        <v>49</v>
+      </c>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B14" s="7">
+        <v>45414</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="8">
+        <v>15</v>
+      </c>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B15" s="7">
+        <v>45417</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="8">
+        <v>13</v>
+      </c>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B16" s="7">
+        <v>45421</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="8">
+        <v>98</v>
+      </c>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B17" s="7">
+        <v>45422</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="8">
+        <v>51</v>
+      </c>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B18" s="7">
+        <v>45422</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="8">
+        <v>66</v>
+      </c>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B19" s="7">
+        <v>45431</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="8">
+        <v>46</v>
+      </c>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B20" s="7">
+        <v>45431</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="8">
+        <v>56</v>
+      </c>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="H24" s="3"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:D20">
+    <sortCondition ref="B4:B20"/>
+  </sortState>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="I1:K1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42537807-2C20-4848-AAA6-DD655807FE37}">
+  <dimension ref="A1:P29"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.75" customWidth="1"/>
+    <col min="5" max="5" width="6.25" customWidth="1"/>
+    <col min="6" max="7" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" customWidth="1"/>
+    <col min="9" max="9" width="11.58203125" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.58203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="I1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4"/>
+      <c r="B2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4"/>
+      <c r="B3" s="7">
+        <v>45377</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="8">
+        <v>67</v>
+      </c>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="I3" s="6">
+        <v>3</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="12">
+        <v>0.5234375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4"/>
+      <c r="B4" s="7">
+        <v>45380</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="8">
+        <v>16</v>
+      </c>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="I4" s="6">
+        <v>3</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="12">
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4"/>
+      <c r="B5" s="7">
+        <v>45380</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="8">
+        <v>21</v>
+      </c>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="I5" s="6">
+        <v>3</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="12">
+        <v>0.2890625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4"/>
+      <c r="B6" s="7">
+        <v>45382</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="8">
+        <v>24</v>
+      </c>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="I6" s="6">
+        <v>4</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="12">
+        <v>0.30456852791878175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4"/>
+      <c r="B7" s="7">
+        <v>45383</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="8">
+        <v>30</v>
+      </c>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="I7" s="6">
+        <v>4</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="12">
+        <v>0.23604060913705585</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B8" s="7">
+        <v>45385</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="8">
+        <v>21</v>
+      </c>
+      <c r="I8" s="6">
+        <v>4</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="12">
+        <v>0.45939086294416243</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B9" s="7">
+        <v>45392</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="8">
+        <v>39</v>
+      </c>
+      <c r="I9" s="6">
+        <v>5</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="12">
+        <v>0.6376811594202898</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B10" s="7">
+        <v>45401</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="8">
+        <v>81</v>
+      </c>
+      <c r="I10" s="6">
+        <v>5</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="12">
+        <v>0.32463768115942027</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B11" s="7">
+        <v>45409</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="8">
+        <v>81</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="6">
+        <v>5</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="12">
+        <v>3.7681159420289857E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B12" s="7">
+        <v>45409</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="8">
+        <v>93</v>
+      </c>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B13" s="7">
+        <v>45410</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="8">
+        <v>49</v>
+      </c>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B14" s="7">
+        <v>45414</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="8">
+        <v>15</v>
+      </c>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B15" s="7">
+        <v>45417</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="8">
+        <v>13</v>
+      </c>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B16" s="7">
+        <v>45421</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="8">
+        <v>98</v>
+      </c>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B17" s="7">
+        <v>45422</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="8">
+        <v>51</v>
+      </c>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B18" s="7">
+        <v>45422</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="8">
+        <v>66</v>
+      </c>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B19" s="7">
+        <v>45431</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="8">
+        <v>46</v>
+      </c>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B20" s="7">
+        <v>45431</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="8">
+        <v>56</v>
+      </c>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="H21" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="F23" cm="1">
+        <f t="array" ref="F23:F25">_xlfn.UNIQUE(MONTH(B3:B20))</f>
+        <v>3</v>
+      </c>
+      <c r="H23" s="15" cm="1">
+        <f t="array" ref="H23:J29">_xlfn._xlws.SORT(_xlfn._xlws.FILTER(B3:D20,MONTH(B3:B20)=H21),3,-1)</f>
+        <v>45409</v>
+      </c>
+      <c r="I23" t="str">
+        <v>F</v>
+      </c>
+      <c r="J23">
+        <v>93</v>
+      </c>
+      <c r="L23" s="14">
+        <f>SUM(_xlfn.TAKE(_xlfn.ANCHORARRAY(H23),,-1))</f>
+        <v>394</v>
+      </c>
+      <c r="N23" t="str" cm="1">
+        <f t="array" ref="N23:P25">_xlfn.LET(_xlpm.z,_xlfn.VSTACK(_xlfn.TAKE(_xlfn.ANCHORARRAY(H23),2,-2),_xlfn.HSTACK("Other",L23-SUM(_xlfn.TAKE(_xlfn.ANCHORARRAY(H23),2,-1)))),_xlpm.z_1,_xlfn.CHOOSECOLS(_xlpm.z,1),_xlpm.z_2,_xlfn.CHOOSECOLS(_xlpm.z,2),_xlfn.EXPAND(_xlfn.HSTACK(_xlpm.z_1,_xlpm.z_2/SUM(_xlpm.z_2)),,3,H21))</f>
+        <v>F</v>
+      </c>
+      <c r="O23">
+        <v>0.23604060913705585</v>
+      </c>
+      <c r="P23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="F24">
+        <v>4</v>
+      </c>
+      <c r="H24" s="15">
+        <v>45401</v>
+      </c>
+      <c r="I24" t="str">
+        <v>E</v>
+      </c>
+      <c r="J24">
+        <v>81</v>
+      </c>
+      <c r="N24" t="str">
+        <v>E</v>
+      </c>
+      <c r="O24">
+        <v>0.20558375634517767</v>
+      </c>
+      <c r="P24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="F25">
+        <v>5</v>
+      </c>
+      <c r="H25" s="14">
+        <v>45409</v>
+      </c>
+      <c r="I25" t="str">
+        <v>D</v>
+      </c>
+      <c r="J25">
+        <v>81</v>
+      </c>
+      <c r="N25" t="str">
+        <v>Other</v>
+      </c>
+      <c r="O25">
+        <v>0.55837563451776651</v>
+      </c>
+      <c r="P25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="H26" s="14">
+        <v>45410</v>
+      </c>
+      <c r="I26" t="str">
+        <v>A</v>
+      </c>
+      <c r="J26">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="H27" s="14">
+        <v>45392</v>
+      </c>
+      <c r="I27" t="str">
+        <v>E</v>
+      </c>
+      <c r="J27">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="H28" s="14">
+        <v>45383</v>
+      </c>
+      <c r="I28" t="str">
+        <v>C</v>
+      </c>
+      <c r="J28">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="H29" s="14">
+        <v>45385</v>
+      </c>
+      <c r="I29" t="str">
+        <v>A</v>
+      </c>
+      <c r="J29">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="I1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{369EB95E-7372-4990-88C5-2D2C844A6F30}">
+  <dimension ref="A1:K33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1172,19 +2270,133 @@
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="H24" s="3"/>
+      <c r="F24" s="9" t="str" cm="1">
+        <f t="array" ref="F24:H33">_xlfn.REDUCE(
+I2:K2,_xlfn.UNIQUE(MONTH(B3:B20)),
+_xlfn.LAMBDA(_xlpm.a,_xlpm.v,
+           _xlfn.VSTACK(_xlpm.a,_xlfn.LET(_xlpm.b,B3:B20,_xlpm.c,C3:C20,_xlpm.d,--(_xlpm.v&amp;-2024),
+                        _xlpm.i,_xlfn.UNIQUE(_xlpm.c),
+                        _xlpm.w,SUMIFS(D3:D20,_xlpm.c,_xlpm.i,_xlpm.b,"&gt;="&amp;_xlpm.d,_xlpm.b,"&lt;"&amp;EDATE(_xlpm.d,1)),
+                        _xlpm.r,_xlfn.IFNA(_xlfn._xlws.SORT(_xlfn.HSTACK(_xlpm.v,_xlpm.i,_xlpm.w/SUM(_xlpm.w)),3,-1),_xlpm.v),
+                        _xlfn.VSTACK(_xlfn.TAKE(_xlpm.r,2),_xlfn.HSTACK(_xlpm.v,"Other",SUM(_xlfn.DROP(_xlpm.r,2,1))))
+                        )
+                 )
+      )
+)</f>
+        <v>Month</v>
+      </c>
+      <c r="G24" s="10" t="str">
+        <v>Product</v>
+      </c>
+      <c r="H24" s="9" t="str">
+        <v>% of Month sales</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F25" s="6">
+        <v>3</v>
+      </c>
+      <c r="G25" s="6" t="str">
+        <v>B</v>
+      </c>
+      <c r="H25" s="12">
+        <v>0.5234375</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F26" s="6">
+        <v>3</v>
+      </c>
+      <c r="G26" s="6" t="str">
+        <v>C</v>
+      </c>
+      <c r="H26" s="12">
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F27" s="6">
+        <v>3</v>
+      </c>
+      <c r="G27" s="6" t="str">
+        <v>Other</v>
+      </c>
+      <c r="H27" s="12">
+        <v>0.2890625</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F28" s="6">
+        <v>4</v>
+      </c>
+      <c r="G28" s="6" t="str">
+        <v>E</v>
+      </c>
+      <c r="H28" s="12">
+        <v>0.30456852791878175</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F29" s="6">
+        <v>4</v>
+      </c>
+      <c r="G29" s="6" t="str">
+        <v>F</v>
+      </c>
+      <c r="H29" s="12">
+        <v>0.23604060913705585</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F30" s="6">
+        <v>4</v>
+      </c>
+      <c r="G30" s="6" t="str">
+        <v>Other</v>
+      </c>
+      <c r="H30" s="12">
+        <v>0.45939086294416243</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F31" s="6">
+        <v>5</v>
+      </c>
+      <c r="G31" s="6" t="str">
+        <v>B</v>
+      </c>
+      <c r="H31" s="12">
+        <v>0.6376811594202898</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F32" s="6">
+        <v>5</v>
+      </c>
+      <c r="G32" s="6" t="str">
+        <v>A</v>
+      </c>
+      <c r="H32" s="12">
+        <v>0.32463768115942027</v>
+      </c>
+    </row>
+    <row r="33" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="F33" s="6">
+        <v>5</v>
+      </c>
+      <c r="G33" s="6" t="str">
+        <v>Other</v>
+      </c>
+      <c r="H33" s="12">
+        <v>3.7681159420289857E-2</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:D20">
-    <sortCondition ref="B4:B20"/>
-  </sortState>
   <mergeCells count="2">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="I1:K1"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Broke down one alternate solution
</commit_message>
<xml_diff>
--- a/CH-96 Top Products.xlsx
+++ b/CH-96 Top Products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28006"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{19F99536-1B9E-419B-A259-9A43C1F93262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2A145DE-BD10-4E9D-9D23-478D6D52AE62}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C4FFCB-23F6-43FE-ACF1-1E5A00CECE8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="22">
   <si>
     <t>Result</t>
   </si>
@@ -113,6 +113,24 @@
   </si>
   <si>
     <t>https://www.linkedin.com/feed/update/urn:li:activity:7228505467411427329/</t>
+  </si>
+  <si>
+    <t>I want to break this down so I understand it.</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>r</t>
   </si>
 </sst>
 </file>
@@ -281,12 +299,12 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -997,37 +1015,37 @@
       <selection activeCell="P12" sqref="O12:P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="4" customWidth="1"/>
-    <col min="2" max="2" width="13.58203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" customWidth="1"/>
-    <col min="4" max="4" width="10.75" customWidth="1"/>
-    <col min="5" max="5" width="6.25" customWidth="1"/>
-    <col min="6" max="7" width="15.83203125" customWidth="1"/>
-    <col min="8" max="8" width="20.83203125" customWidth="1"/>
-    <col min="9" max="9" width="11.58203125" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" customWidth="1"/>
+    <col min="6" max="7" width="15.77734375" customWidth="1"/>
+    <col min="8" max="8" width="20.77734375" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.58203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="I1" s="13" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="I1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
       <c r="N1" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="9" t="s">
         <v>6</v>
@@ -1049,7 +1067,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="7">
         <v>45377</v>
@@ -1073,7 +1091,7 @@
         <v>0.5234375</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="7">
         <v>45380</v>
@@ -1097,7 +1115,7 @@
         <v>0.1875</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="7">
         <v>45380</v>
@@ -1121,7 +1139,7 @@
         <v>0.2890625</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="7">
         <v>45382</v>
@@ -1145,7 +1163,7 @@
         <v>0.30456852791878175</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="7">
         <v>45383</v>
@@ -1169,7 +1187,7 @@
         <v>0.23604060913705585</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8" s="7">
         <v>45385</v>
       </c>
@@ -1189,7 +1207,7 @@
         <v>0.45939086294416243</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
         <v>45392</v>
       </c>
@@ -1209,7 +1227,7 @@
         <v>0.6376811594202898</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" s="7">
         <v>45401</v>
       </c>
@@ -1229,7 +1247,7 @@
         <v>0.32463768115942027</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
         <v>45409</v>
       </c>
@@ -1250,7 +1268,7 @@
         <v>3.7681159420289857E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
         <v>45409</v>
       </c>
@@ -1262,7 +1280,7 @@
       </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B13" s="7">
         <v>45410</v>
       </c>
@@ -1274,7 +1292,7 @@
       </c>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" s="7">
         <v>45414</v>
       </c>
@@ -1286,7 +1304,7 @@
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B15" s="7">
         <v>45417</v>
       </c>
@@ -1298,7 +1316,7 @@
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" s="7">
         <v>45421</v>
       </c>
@@ -1310,7 +1328,7 @@
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="7">
         <v>45422</v>
       </c>
@@ -1322,7 +1340,7 @@
       </c>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="7">
         <v>45422</v>
       </c>
@@ -1334,7 +1352,7 @@
       </c>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="7">
         <v>45431</v>
       </c>
@@ -1346,7 +1364,7 @@
       </c>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="7">
         <v>45431</v>
       </c>
@@ -1358,16 +1376,16 @@
       </c>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H24" s="3"/>
     </row>
   </sheetData>
@@ -1393,35 +1411,35 @@
       <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="4" customWidth="1"/>
-    <col min="2" max="2" width="13.58203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" customWidth="1"/>
-    <col min="4" max="4" width="10.75" customWidth="1"/>
-    <col min="5" max="5" width="6.25" customWidth="1"/>
-    <col min="6" max="7" width="15.83203125" customWidth="1"/>
-    <col min="8" max="8" width="20.83203125" customWidth="1"/>
-    <col min="9" max="9" width="11.58203125" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" customWidth="1"/>
+    <col min="6" max="7" width="15.77734375" customWidth="1"/>
+    <col min="8" max="8" width="20.77734375" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.58203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="I1" s="13" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="I1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="9" t="s">
         <v>6</v>
@@ -1443,7 +1461,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="7">
         <v>45377</v>
@@ -1467,7 +1485,7 @@
         <v>0.5234375</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="7">
         <v>45380</v>
@@ -1491,7 +1509,7 @@
         <v>0.1875</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="7">
         <v>45380</v>
@@ -1515,7 +1533,7 @@
         <v>0.2890625</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="7">
         <v>45382</v>
@@ -1539,7 +1557,7 @@
         <v>0.30456852791878175</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="7">
         <v>45383</v>
@@ -1563,7 +1581,7 @@
         <v>0.23604060913705585</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" s="7">
         <v>45385</v>
       </c>
@@ -1583,7 +1601,7 @@
         <v>0.45939086294416243</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
         <v>45392</v>
       </c>
@@ -1603,7 +1621,7 @@
         <v>0.6376811594202898</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" s="7">
         <v>45401</v>
       </c>
@@ -1623,7 +1641,7 @@
         <v>0.32463768115942027</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
         <v>45409</v>
       </c>
@@ -1644,7 +1662,7 @@
         <v>3.7681159420289857E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
         <v>45409</v>
       </c>
@@ -1656,7 +1674,7 @@
       </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" s="7">
         <v>45410</v>
       </c>
@@ -1668,7 +1686,7 @@
       </c>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" s="7">
         <v>45414</v>
       </c>
@@ -1680,7 +1698,7 @@
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" s="7">
         <v>45417</v>
       </c>
@@ -1692,7 +1710,7 @@
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" s="7">
         <v>45421</v>
       </c>
@@ -1704,7 +1722,7 @@
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B17" s="7">
         <v>45422</v>
       </c>
@@ -1716,7 +1734,7 @@
       </c>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B18" s="7">
         <v>45422</v>
       </c>
@@ -1728,7 +1746,7 @@
       </c>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B19" s="7">
         <v>45431</v>
       </c>
@@ -1740,7 +1758,7 @@
       </c>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20" s="7">
         <v>45431</v>
       </c>
@@ -1752,23 +1770,23 @@
       </c>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="H21" s="15">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="H21" s="14">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
       <c r="F22" t="s">
         <v>14</v>
       </c>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
       <c r="F23" cm="1">
         <f t="array" ref="F23:F25">_xlfn.UNIQUE(MONTH(B3:B20))</f>
         <v>3</v>
       </c>
-      <c r="H23" s="15" cm="1">
+      <c r="H23" s="14" cm="1">
         <f t="array" ref="H23:J29">_xlfn._xlws.SORT(_xlfn._xlws.FILTER(B3:D20,MONTH(B3:B20)=H21),3,-1)</f>
         <v>45409</v>
       </c>
@@ -1778,7 +1796,7 @@
       <c r="J23">
         <v>93</v>
       </c>
-      <c r="L23" s="14">
+      <c r="L23" s="13">
         <f>SUM(_xlfn.TAKE(_xlfn.ANCHORARRAY(H23),,-1))</f>
         <v>394</v>
       </c>
@@ -1793,11 +1811,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
       <c r="F24">
         <v>4</v>
       </c>
-      <c r="H24" s="15">
+      <c r="H24" s="14">
         <v>45401</v>
       </c>
       <c r="I24" t="str">
@@ -1816,11 +1834,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
       <c r="F25">
         <v>5</v>
       </c>
-      <c r="H25" s="14">
+      <c r="H25" s="13">
         <v>45409</v>
       </c>
       <c r="I25" t="str">
@@ -1839,8 +1857,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="H26" s="14">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="H26" s="13">
         <v>45410</v>
       </c>
       <c r="I26" t="str">
@@ -1850,8 +1868,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="H27" s="14">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="H27" s="13">
         <v>45392</v>
       </c>
       <c r="I27" t="str">
@@ -1861,8 +1879,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="H28" s="14">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="H28" s="13">
         <v>45383</v>
       </c>
       <c r="I28" t="str">
@@ -1872,8 +1890,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="H29" s="14">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="H29" s="13">
         <v>45385</v>
       </c>
       <c r="I29" t="str">
@@ -1896,40 +1914,40 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{369EB95E-7372-4990-88C5-2D2C844A6F30}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="C18" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="4" customWidth="1"/>
-    <col min="2" max="2" width="13.58203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" customWidth="1"/>
-    <col min="4" max="4" width="10.75" customWidth="1"/>
-    <col min="5" max="5" width="6.25" customWidth="1"/>
-    <col min="6" max="7" width="15.83203125" customWidth="1"/>
-    <col min="8" max="8" width="20.83203125" customWidth="1"/>
-    <col min="9" max="9" width="11.58203125" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" customWidth="1"/>
+    <col min="6" max="7" width="15.77734375" customWidth="1"/>
+    <col min="8" max="8" width="20.77734375" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.58203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="I1" s="13" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="I1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="9" t="s">
         <v>6</v>
@@ -1951,7 +1969,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="7">
         <v>45377</v>
@@ -1975,7 +1993,7 @@
         <v>0.5234375</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="7">
         <v>45380</v>
@@ -1999,7 +2017,7 @@
         <v>0.1875</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="7">
         <v>45380</v>
@@ -2023,7 +2041,7 @@
         <v>0.2890625</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="7">
         <v>45382</v>
@@ -2047,7 +2065,7 @@
         <v>0.30456852791878175</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="7">
         <v>45383</v>
@@ -2071,7 +2089,7 @@
         <v>0.23604060913705585</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" s="7">
         <v>45385</v>
       </c>
@@ -2091,7 +2109,7 @@
         <v>0.45939086294416243</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
         <v>45392</v>
       </c>
@@ -2111,7 +2129,7 @@
         <v>0.6376811594202898</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" s="7">
         <v>45401</v>
       </c>
@@ -2131,7 +2149,7 @@
         <v>0.32463768115942027</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
         <v>45409</v>
       </c>
@@ -2152,7 +2170,7 @@
         <v>3.7681159420289857E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
         <v>45409</v>
       </c>
@@ -2164,7 +2182,7 @@
       </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" s="7">
         <v>45410</v>
       </c>
@@ -2176,7 +2194,7 @@
       </c>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" s="7">
         <v>45414</v>
       </c>
@@ -2188,7 +2206,7 @@
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" s="7">
         <v>45417</v>
       </c>
@@ -2200,7 +2218,7 @@
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" s="7">
         <v>45421</v>
       </c>
@@ -2212,7 +2230,7 @@
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B17" s="7">
         <v>45422</v>
       </c>
@@ -2224,7 +2242,7 @@
       </c>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B18" s="7">
         <v>45422</v>
       </c>
@@ -2236,7 +2254,7 @@
       </c>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B19" s="7">
         <v>45431</v>
       </c>
@@ -2247,8 +2265,11 @@
         <v>46</v>
       </c>
       <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B20" s="7">
         <v>45431</v>
       </c>
@@ -2260,16 +2281,28 @@
       </c>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.3">
       <c r="H21" s="3"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="L21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.3">
       <c r="H22" s="3"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="K22" t="s">
+        <v>11</v>
+      </c>
+      <c r="L22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.3">
       <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="J23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.3">
       <c r="F24" s="9" t="str" cm="1">
         <f t="array" ref="F24:H33">_xlfn.REDUCE(
 I2:K2,_xlfn.UNIQUE(MONTH(B3:B20)),
@@ -2291,8 +2324,20 @@
       <c r="H24" s="9" t="str">
         <v>% of Month sales</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="J24" t="s">
+        <v>4</v>
+      </c>
+      <c r="K24" t="s">
+        <v>19</v>
+      </c>
+      <c r="L24" t="s">
+        <v>18</v>
+      </c>
+      <c r="N24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.3">
       <c r="F25" s="6">
         <v>3</v>
       </c>
@@ -2302,8 +2347,40 @@
       <c r="H25" s="12">
         <v>0.5234375</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="J25" t="str" cm="1">
+        <f t="array" ref="J25:J30">_xlfn._xlws.SORT(_xlfn.UNIQUE(C3:C20))</f>
+        <v>A</v>
+      </c>
+      <c r="K25">
+        <f>--(L22&amp;-2024)</f>
+        <v>45413</v>
+      </c>
+      <c r="L25" cm="1">
+        <f t="array" ref="L25:L30">SUMIFS(D3:D20,C3:C20,_xlfn.ANCHORARRAY(J25),B3:B20,"&gt;="&amp;K25,B3:B20,"&lt;"&amp;EDATE(K25,1))</f>
+        <v>112</v>
+      </c>
+      <c r="N25" cm="1">
+        <f t="array" ref="N25:P30">_xlfn.IFNA(_xlfn._xlws.SORT(_xlfn.HSTACK($L$22,_xlfn.ANCHORARRAY($J$25),_xlfn.ANCHORARRAY($L$25)/SUM(_xlfn.ANCHORARRAY($L$25))),3,-1),$L$22)</f>
+        <v>5</v>
+      </c>
+      <c r="O25" t="str">
+        <v>B</v>
+      </c>
+      <c r="P25">
+        <v>0.6376811594202898</v>
+      </c>
+      <c r="R25" cm="1">
+        <f t="array" ref="R25:T27">_xlfn.VSTACK(_xlfn.TAKE(_xlfn.ANCHORARRAY(N25),2),_xlfn.HSTACK(L22,"Other",SUM(_xlfn.DROP(_xlfn.ANCHORARRAY(N25),2,1))))</f>
+        <v>5</v>
+      </c>
+      <c r="S25" t="str">
+        <v>B</v>
+      </c>
+      <c r="T25">
+        <v>0.6376811594202898</v>
+      </c>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.3">
       <c r="F26" s="6">
         <v>3</v>
       </c>
@@ -2313,8 +2390,32 @@
       <c r="H26" s="12">
         <v>0.1875</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="J26" t="str">
+        <v>B</v>
+      </c>
+      <c r="L26">
+        <v>220</v>
+      </c>
+      <c r="N26">
+        <v>5</v>
+      </c>
+      <c r="O26" t="str">
+        <v>A</v>
+      </c>
+      <c r="P26">
+        <v>0.32463768115942027</v>
+      </c>
+      <c r="R26">
+        <v>5</v>
+      </c>
+      <c r="S26" t="str">
+        <v>A</v>
+      </c>
+      <c r="T26">
+        <v>0.32463768115942027</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.3">
       <c r="F27" s="6">
         <v>3</v>
       </c>
@@ -2324,8 +2425,32 @@
       <c r="H27" s="12">
         <v>0.2890625</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="J27" t="str">
+        <v>C</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>5</v>
+      </c>
+      <c r="O27" t="str">
+        <v>F</v>
+      </c>
+      <c r="P27">
+        <v>3.7681159420289857E-2</v>
+      </c>
+      <c r="R27">
+        <v>5</v>
+      </c>
+      <c r="S27" t="str">
+        <v>Other</v>
+      </c>
+      <c r="T27">
+        <v>3.7681159420289857E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.3">
       <c r="F28" s="6">
         <v>4</v>
       </c>
@@ -2335,8 +2460,23 @@
       <c r="H28" s="12">
         <v>0.30456852791878175</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="J28" t="str">
+        <v>D</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>5</v>
+      </c>
+      <c r="O28" t="str">
+        <v>C</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.3">
       <c r="F29" s="6">
         <v>4</v>
       </c>
@@ -2346,8 +2486,23 @@
       <c r="H29" s="12">
         <v>0.23604060913705585</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="J29" t="str">
+        <v>E</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>5</v>
+      </c>
+      <c r="O29" t="str">
+        <v>D</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.3">
       <c r="F30" s="6">
         <v>4</v>
       </c>
@@ -2357,8 +2512,23 @@
       <c r="H30" s="12">
         <v>0.45939086294416243</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="J30" t="str">
+        <v>F</v>
+      </c>
+      <c r="L30">
+        <v>13</v>
+      </c>
+      <c r="N30">
+        <v>5</v>
+      </c>
+      <c r="O30" t="str">
+        <v>E</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.3">
       <c r="F31" s="6">
         <v>5</v>
       </c>
@@ -2369,7 +2539,7 @@
         <v>0.6376811594202898</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:20" x14ac:dyDescent="0.3">
       <c r="F32" s="6">
         <v>5</v>
       </c>
@@ -2380,7 +2550,7 @@
         <v>0.32463768115942027</v>
       </c>
     </row>
-    <row r="33" spans="6:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F33" s="6">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Broke down second alternative
</commit_message>
<xml_diff>
--- a/CH-96 Top Products.xlsx
+++ b/CH-96 Top Products.xlsx
@@ -8,19 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C4FFCB-23F6-43FE-ACF1-1E5A00CECE8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5935F2FB-52F4-45A6-9158-7DDEBBCB7CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="Alt1" sheetId="3" r:id="rId3"/>
+    <sheet name="Alt2" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt1'!$B$2:$D$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Alt2'!$B$2:$D$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$D$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$D$16</definedName>
+    <definedName name="_g">'Alt2'!$G$24:$H$27</definedName>
+    <definedName name="_h">'Alt2'!$I$24:$J$25</definedName>
+    <definedName name="_k">'Alt2'!$L$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="25">
   <si>
     <t>Result</t>
   </si>
@@ -132,12 +137,24 @@
   <si>
     <t>r</t>
   </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0;\-0;0;@"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +180,14 @@
       <color theme="1"/>
       <name val="Trebuchet MS"/>
       <family val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -262,10 +287,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -306,8 +332,16 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1007,12 +1041,39 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="883" row="9">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{A82AB5BD-0334-4663-A757-E44F35899BC0}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P12" sqref="O12:P12"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1041,7 +1102,7 @@
       </c>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="16" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1397,9 +1458,12 @@
     <mergeCell ref="I1:K1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="N1" r:id="rId1" xr:uid="{9F3B9EC1-56E4-466D-9227-AA150001B36C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1407,7 +1471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42537807-2C20-4848-AAA6-DD655807FE37}">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B6" workbookViewId="0">
       <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
@@ -1916,8 +1980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{369EB95E-7372-4990-88C5-2D2C844A6F30}">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C18" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2569,4 +2633,648 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D491D338-1E98-4147-B292-6BFE9CC7642E}">
+  <dimension ref="A1:N33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" customWidth="1"/>
+    <col min="7" max="7" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="I1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="N1" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="7">
+        <v>45377</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="8">
+        <v>67</v>
+      </c>
+      <c r="E3"/>
+      <c r="F3" cm="1">
+        <f t="array" ref="F3:F20">MONTH(B3:B20)</f>
+        <v>3</v>
+      </c>
+      <c r="G3"/>
+      <c r="I3" s="6">
+        <v>3</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="12">
+        <v>0.5234375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="7">
+        <v>45380</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="8">
+        <v>16</v>
+      </c>
+      <c r="E4"/>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4"/>
+      <c r="I4" s="6">
+        <v>3</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="12">
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="7">
+        <v>45380</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="8">
+        <v>21</v>
+      </c>
+      <c r="E5"/>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5"/>
+      <c r="I5" s="6">
+        <v>3</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="12">
+        <v>0.2890625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="7">
+        <v>45382</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="8">
+        <v>24</v>
+      </c>
+      <c r="E6"/>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6"/>
+      <c r="I6" s="6">
+        <v>4</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="12">
+        <v>0.30456852791878175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="7">
+        <v>45383</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="8">
+        <v>30</v>
+      </c>
+      <c r="E7"/>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7"/>
+      <c r="I7" s="6">
+        <v>4</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="12">
+        <v>0.23604060913705585</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B8" s="7">
+        <v>45385</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="8">
+        <v>21</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="I8" s="6">
+        <v>4</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="12">
+        <v>0.45939086294416243</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B9" s="7">
+        <v>45392</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="8">
+        <v>39</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="I9" s="6">
+        <v>5</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="12">
+        <v>0.6376811594202898</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B10" s="7">
+        <v>45401</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="8">
+        <v>81</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="I10" s="6">
+        <v>5</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="12">
+        <v>0.32463768115942027</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B11" s="7">
+        <v>45409</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="8">
+        <v>81</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="6">
+        <v>5</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="12">
+        <v>3.7681159420289857E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B12" s="7">
+        <v>45409</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="8">
+        <v>93</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13" s="7">
+        <v>45410</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="8">
+        <v>49</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14" s="7">
+        <v>45414</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="8">
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15" s="7">
+        <v>45417</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="8">
+        <v>13</v>
+      </c>
+      <c r="F15">
+        <v>5</v>
+      </c>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B16" s="7">
+        <v>45421</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="8">
+        <v>98</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B17" s="7">
+        <v>45422</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="8">
+        <v>51</v>
+      </c>
+      <c r="F17">
+        <v>5</v>
+      </c>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B18" s="7">
+        <v>45422</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="8">
+        <v>66</v>
+      </c>
+      <c r="F18">
+        <v>5</v>
+      </c>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B19" s="7">
+        <v>45431</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="8">
+        <v>46</v>
+      </c>
+      <c r="F19">
+        <v>5</v>
+      </c>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B20" s="7">
+        <v>45431</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="8">
+        <v>56</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="3"/>
+      <c r="I23" t="s">
+        <v>23</v>
+      </c>
+      <c r="L23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C24" t="str" cm="1">
+        <f t="array" ref="C24:E33">_xlfn.LET(
+    _xlpm.m, MONTH(B3:B20),
+    _xlpm.p, C3:C20,
+    _xlpm.q, D3:D20,
+    _xlfn.REDUCE(
+        I2:K2,
+        _xlfn.UNIQUE(_xlpm.m),
+        _xlfn.LAMBDA(_xlpm.a,_xlpm.i,
+            _xlfn.LET(
+                _xlpm.g, _xlfn.GROUPBY(_xlpm.p, _xlpm.q, _xleta.SUM, , 0, -2, _xlpm.m = _xlpm.i),
+                _xlpm.h, _xlfn.TAKE(_xlpm.g, 2),
+                _xlpm.k, IFERROR(_xlpm.h / SUM(_xlpm.g), _xlpm.h),
+                _xlfn.VSTACK(
+                    _xlpm.a,
+                    _xlfn.IFNA(_xlfn.HSTACK(_xlpm.i, _xlfn.VSTACK(_xlpm.k, _xlfn.HSTACK("Other", 1 - SUM(_xlpm.k)))), _xlpm.i)
+                )
+            )
+        )
+    )
+)</f>
+        <v>Month</v>
+      </c>
+      <c r="D24" t="str">
+        <v>Product</v>
+      </c>
+      <c r="E24" t="str">
+        <v>% of Month sales</v>
+      </c>
+      <c r="G24" s="17" t="str" cm="1">
+        <f t="array" ref="G24:H27">_xlfn.GROUPBY(C3:C20,D3:D20, _xleta.SUM, , 0, -2,_xlfn.ANCHORARRAY(F3)=H21)</f>
+        <v>B</v>
+      </c>
+      <c r="H24">
+        <v>67</v>
+      </c>
+      <c r="I24" t="str" cm="1">
+        <f t="array" ref="I24:J25">_xlfn.TAKE(_g,2)</f>
+        <v>B</v>
+      </c>
+      <c r="J24">
+        <v>67</v>
+      </c>
+      <c r="L24" t="str" cm="1">
+        <f t="array" ref="L24:M25">IFERROR(_h/SUM(_g),_h)</f>
+        <v>B</v>
+      </c>
+      <c r="M24">
+        <v>0.5234375</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25" t="str">
+        <v>B</v>
+      </c>
+      <c r="E25">
+        <v>0.5234375</v>
+      </c>
+      <c r="G25" t="str">
+        <v>C</v>
+      </c>
+      <c r="H25">
+        <v>24</v>
+      </c>
+      <c r="I25" t="str">
+        <v>C</v>
+      </c>
+      <c r="J25">
+        <v>24</v>
+      </c>
+      <c r="L25" t="str">
+        <v>C</v>
+      </c>
+      <c r="M25">
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26" t="str">
+        <v>C</v>
+      </c>
+      <c r="E26">
+        <v>0.1875</v>
+      </c>
+      <c r="G26" t="str">
+        <v>D</v>
+      </c>
+      <c r="H26">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" t="str">
+        <v>Other</v>
+      </c>
+      <c r="E27">
+        <v>0.2890625</v>
+      </c>
+      <c r="G27" t="str">
+        <v>A</v>
+      </c>
+      <c r="H27">
+        <v>16</v>
+      </c>
+      <c r="L27" t="str" cm="1">
+        <f t="array" ref="L27:M27">_xlfn.HSTACK("Other",1-SUM(_xlfn.ANCHORARRAY(_k)))</f>
+        <v>Other</v>
+      </c>
+      <c r="M27">
+        <v>0.2890625</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28" t="str">
+        <v>E</v>
+      </c>
+      <c r="E28">
+        <v>0.30456852791878175</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29" t="str">
+        <v>F</v>
+      </c>
+      <c r="E29">
+        <v>0.23604060913705585</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30" t="str">
+        <v>Other</v>
+      </c>
+      <c r="E30">
+        <v>0.45939086294416243</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31" t="str">
+        <v>B</v>
+      </c>
+      <c r="E31">
+        <v>0.6376811594202898</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>5</v>
+      </c>
+      <c r="D32" t="str">
+        <v>A</v>
+      </c>
+      <c r="E32">
+        <v>0.32463768115942027</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>5</v>
+      </c>
+      <c r="D33" t="str">
+        <v>Other</v>
+      </c>
+      <c r="E33">
+        <v>3.7681159420289934E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="I1:K1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="N1" r:id="rId1" xr:uid="{8D3C26B6-3E79-46E2-B775-660E5AAB19F4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>